<commit_message>
Update release plan docs
</commit_message>
<xml_diff>
--- a/Working/01_Documents/11_Preliminary Release Plan.xlsx
+++ b/Working/01_Documents/11_Preliminary Release Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215"/>
+    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
-  <si>
-    <t>PRODUCT BACKLOG</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+  <si>
+    <t>RELEASE PLAN</t>
   </si>
   <si>
     <t>ID</t>
@@ -127,9 +127,6 @@
   <si>
     <t>Thống kê, kiểm toán doanh thu có được theo từng rạp,
 cụm rạp, từng phim hoặc từng ngày</t>
-  </si>
-  <si>
-    <t>Product Backlog</t>
   </si>
   <si>
     <t>Actor</t>
@@ -167,10 +164,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -241,6 +238,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -249,30 +268,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,9 +299,54 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,7 +361,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,67 +370,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,37 +403,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,19 +433,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,13 +475,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,19 +523,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,55 +571,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,11 +600,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,7 +643,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,32 +659,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -695,23 +681,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -721,130 +718,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1181,7 +1178,7 @@
   <sheetPr/>
   <dimension ref="A1:F996"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -2514,8 +2511,8 @@
   <sheetPr/>
   <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2530,7 +2527,7 @@
   <sheetData>
     <row r="1" ht="22.8" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2542,10 +2539,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>5</v>
@@ -2559,10 +2556,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="D3" s="8">
         <v>1</v>
@@ -2576,10 +2573,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -2589,10 +2586,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2602,10 +2599,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
@@ -2619,10 +2616,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -2632,10 +2629,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -2645,10 +2642,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
@@ -2662,10 +2659,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>

</xml_diff>

<commit_message>
Update date in docs
</commit_message>
<xml_diff>
--- a/Working/01_Documents/11_Preliminary Release Plan.xlsx
+++ b/Working/01_Documents/11_Preliminary Release Plan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longmv\Desktop\HCMUS\Software_Process\QTPM2022\Working\01_Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>RELEASE PLAN</t>
   </si>
@@ -157,19 +162,40 @@
   </si>
   <si>
     <t>Tôi muốn có tài liệu hướng dẫn sử dụng sản phẩm</t>
+  </si>
+  <si>
+    <t>12/3/2022</t>
+  </si>
+  <si>
+    <t>12/10/2022</t>
+  </si>
+  <si>
+    <t>12/17/2022</t>
+  </si>
+  <si>
+    <t>10/8/2022</t>
+  </si>
+  <si>
+    <t>10/15/2022</t>
+  </si>
+  <si>
+    <t>10/29/2022</t>
+  </si>
+  <si>
+    <t>11/4/2022</t>
+  </si>
+  <si>
+    <t>11/12/2022</t>
+  </si>
+  <si>
+    <t>11/26/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,346 +263,16 @@
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -599,257 +295,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -866,12 +317,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -885,19 +330,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -917,62 +350,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1170,356 +583,356 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F996"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13" style="13" customWidth="1"/>
-    <col min="3" max="3" width="47" style="13" customWidth="1"/>
-    <col min="4" max="4" width="54.5740740740741" style="13" customWidth="1"/>
-    <col min="5" max="5" width="22.1111111111111" style="13" customWidth="1"/>
-    <col min="6" max="6" width="16.2222222222222" style="13" customWidth="1"/>
-    <col min="7" max="23" width="9" style="13" customWidth="1"/>
-    <col min="24" max="16384" width="14.4259259259259" style="13"/>
+    <col min="1" max="1" width="4" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13" style="10" customWidth="1"/>
+    <col min="3" max="3" width="47" style="10" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="10" customWidth="1"/>
+    <col min="7" max="23" width="9" style="10" customWidth="1"/>
+    <col min="24" max="16384" width="14.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.8" spans="1:6">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:6" ht="22.5">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" ht="19" customHeight="1" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.95" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A3" s="16">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="21">
         <v>1</v>
       </c>
-      <c r="F3" s="18">
-        <v>44842</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A4" s="16">
+      <c r="F3" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A5" s="16">
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A6" s="16">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="21">
         <v>1</v>
       </c>
-      <c r="F6" s="18">
-        <v>44849</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A7" s="16">
+      <c r="F6" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A8" s="16">
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="21">
         <v>2</v>
       </c>
-      <c r="F8" s="18">
-        <v>44863</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A9" s="16">
+      <c r="F8" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A10" s="16">
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A11" s="16">
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="21">
         <v>1</v>
       </c>
-      <c r="F11" s="18">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A12" s="16">
+      <c r="F11" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A13" s="16">
+      <c r="E12" s="21"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="21">
         <v>2</v>
       </c>
-      <c r="F13" s="18">
-        <v>44877</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A14" s="16">
+      <c r="F13" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A15" s="16">
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A15" s="12">
         <v>13</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="21">
         <v>2</v>
       </c>
-      <c r="F15" s="18">
-        <v>44891</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A16" s="16">
+      <c r="F15" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A16" s="12">
         <v>14</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A17" s="16">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A17" s="12">
         <v>15</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" s="13" customFormat="1" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-    </row>
-    <row r="19" s="14" customFormat="1" ht="14.25" customHeight="1" spans="5:5">
-      <c r="E19" s="24"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="18" spans="3:4">
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-    </row>
-    <row r="22" ht="18" spans="3:4">
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-    </row>
-    <row r="23" ht="18" spans="3:4">
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" s="11" customFormat="1" ht="14.25" customHeight="1">
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:6" ht="18.75">
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75">
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75">
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2486,11 +1899,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="F3:F5"/>
@@ -2499,183 +1907,186 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="43" orientation="landscape"/>
-  <headerFooter/>
+  <pageSetup scale="43" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.44444444444444" customWidth="1"/>
-    <col min="2" max="2" width="12.712962962963" customWidth="1"/>
-    <col min="3" max="3" width="68.8611111111111" customWidth="1"/>
-    <col min="4" max="4" width="21.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="16.2222222222222" customWidth="1"/>
-    <col min="6" max="27" width="8.86111111111111" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="27" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.8" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="22.5">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" ht="17.4" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A3" s="5">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="25">
         <v>1</v>
       </c>
-      <c r="E3" s="9">
-        <v>44898</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A4" s="5">
+      <c r="E3" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A5" s="5">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A6" s="5">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="25">
         <v>1</v>
       </c>
-      <c r="E6" s="9">
-        <v>44905</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A7" s="5">
+      <c r="E6" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A8" s="5">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A9" s="5">
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="25">
         <v>1</v>
       </c>
-      <c r="E9" s="9">
-        <v>44912</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A10" s="5">
+      <c r="E9" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1">
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3667,7 +3078,6 @@
     <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="92" orientation="landscape"/>
-  <headerFooter/>
+  <pageSetup scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>